<commit_message>
Settling on Roles rather than Joins
</commit_message>
<xml_diff>
--- a/backend/test/data/import-sample.xlsx
+++ b/backend/test/data/import-sample.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikewong899/devel/shinsa/backend/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DA78C62-DF90-B143-A524-6836FA15BA92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6617330-E5C4-9942-A36B-FEA0D415C71B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9460" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{AA8BA195-F7AF-1947-91E7-B7BBD1D6DD1A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Examinees" sheetId="1" r:id="rId1"/>
+    <sheet name="Examiners" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>1st Dan Candidates</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>First Name</t>
   </si>
@@ -49,6 +47,12 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>New Rank</t>
   </si>
 </sst>
 </file>
@@ -400,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3EC8E6-12CD-5546-91A0-05FAE5C3950F}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,35 +415,48 @@
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B738626D-3947-0841-9FCF-0778814271A4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding network health monitoring
</commit_message>
<xml_diff>
--- a/backend/test/data/import-sample.xlsx
+++ b/backend/test/data/import-sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikewong899/devel/shinsa/backend/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6617330-E5C4-9942-A36B-FEA0D415C71B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982FC0AD-67F5-AA4B-B984-C599833E5F5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{AA8BA195-F7AF-1947-91E7-B7BBD1D6DD1A}"/>
+    <workbookView xWindow="9460" yWindow="2080" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA8BA195-F7AF-1947-91E7-B7BBD1D6DD1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Examinees" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>First Name</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>New Rank</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
@@ -404,18 +410,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3EC8E6-12CD-5546-91A0-05FAE5C3950F}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -435,12 +441,18 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -451,12 +463,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B738626D-3947-0841-9FCF-0778814271A4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>